<commit_message>
cambios para proteger ruteo, lista con todos y escond
</commit_message>
<xml_diff>
--- a/Pagos.xlsx
+++ b/Pagos.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,13 +415,13 @@
         <v>fecha</v>
       </c>
       <c r="B1" t="str">
+        <v>folio</v>
+      </c>
+      <c r="C1" t="str">
         <v>mensualidad</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>refPago</v>
-      </c>
-      <c r="D1" t="str">
-        <v>folio</v>
       </c>
       <c r="E1" t="str">
         <v>refBanco</v>
@@ -435,19 +435,19 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>44511.74958333333</v>
+        <v>44544.74958333333</v>
       </c>
       <c r="B2">
-        <v>2430</v>
-      </c>
-      <c r="C2" t="str">
-        <v>mensualidad noviembre</v>
-      </c>
-      <c r="D2">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>4673</v>
+      </c>
+      <c r="D2" t="str">
+        <v>mensualidad diciembre</v>
       </c>
       <c r="E2" t="str">
-        <v>5687</v>
+        <v>5737</v>
       </c>
       <c r="F2" t="str">
         <v>1118668575</v>
@@ -458,19 +458,19 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>44542.74958333333</v>
+        <v>44544.74958333333</v>
       </c>
       <c r="B3">
-        <v>2430</v>
-      </c>
-      <c r="C3" t="str">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>3608</v>
+      </c>
+      <c r="D3" t="str">
         <v>mensualidad diciembre</v>
       </c>
-      <c r="D3">
-        <v>15</v>
-      </c>
       <c r="E3" t="str">
-        <v>5687</v>
+        <v>5713</v>
       </c>
       <c r="F3" t="str">
         <v>1118668575</v>
@@ -481,19 +481,19 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>44577.74958333333</v>
+        <v>44581.74958333333</v>
       </c>
       <c r="B4">
-        <v>2430</v>
-      </c>
-      <c r="C4" t="str">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>3608</v>
+      </c>
+      <c r="D4" t="str">
         <v>MENSUALIDAD ENERO 2022</v>
       </c>
-      <c r="D4">
-        <v>16</v>
-      </c>
       <c r="E4" t="str">
-        <v>5687 - 5813</v>
+        <v>6562</v>
       </c>
       <c r="F4" t="str">
         <v>1118668575</v>
@@ -504,19 +504,19 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>44615.74958333333</v>
+        <v>44581.74958333333</v>
       </c>
       <c r="B5">
-        <v>2430</v>
-      </c>
-      <c r="C5" t="str">
-        <v>mensualidad febrero 2022</v>
-      </c>
-      <c r="D5">
-        <v>17</v>
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>4673</v>
+      </c>
+      <c r="D5" t="str">
+        <v>MENSUALIDAD ENERO 2022</v>
       </c>
       <c r="E5" t="str">
-        <v>6313</v>
+        <v>6563</v>
       </c>
       <c r="F5" t="str">
         <v>1118668575</v>
@@ -527,19 +527,19 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>44643.74958333333</v>
+        <v>44612.74958333333</v>
       </c>
       <c r="B6">
-        <v>2430</v>
-      </c>
-      <c r="C6" t="str">
-        <v>mensualidad marzo 2022</v>
-      </c>
-      <c r="D6">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>4673</v>
+      </c>
+      <c r="D6" t="str">
+        <v>mensualidad febrero 2022</v>
       </c>
       <c r="E6" t="str">
-        <v>7211</v>
+        <v>7149</v>
       </c>
       <c r="F6" t="str">
         <v>1118668575</v>
@@ -550,19 +550,19 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>44676.79125</v>
+        <v>44612.74958333333</v>
       </c>
       <c r="B7">
-        <v>2430</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Mensualidad Abril 2022</v>
-      </c>
-      <c r="D7">
-        <v>19</v>
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>3608</v>
+      </c>
+      <c r="D7" t="str">
+        <v>mensualidad febrero 2022</v>
       </c>
       <c r="E7" t="str">
-        <v xml:space="preserve"> Se toman a cuenta 224 del saldo a favor de febrero y se cubre con el num de mov9142</v>
+        <v>7148</v>
       </c>
       <c r="F7" t="str">
         <v>1118668575</v>
@@ -573,19 +573,19 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>44706.79125</v>
+        <v>44641.74958333333</v>
       </c>
       <c r="B8">
-        <v>2430</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Mensualidad Mayo 2022</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>4673</v>
+      </c>
+      <c r="D8" t="str">
+        <v>mensualidad marzo 2022</v>
       </c>
       <c r="E8" t="str">
-        <v>9142</v>
+        <v>7790</v>
       </c>
       <c r="F8" t="str">
         <v>1118668575</v>
@@ -596,19 +596,19 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>44741.79125</v>
+        <v>44641.74958333333</v>
       </c>
       <c r="B9">
-        <v>2430</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Mensualidad Junio 2022</v>
-      </c>
-      <c r="D9">
-        <v>21</v>
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>3608</v>
+      </c>
+      <c r="D9" t="str">
+        <v>mensualidad marzo 2022</v>
       </c>
       <c r="E9" t="str">
-        <v>10050</v>
+        <v>7789</v>
       </c>
       <c r="F9" t="str">
         <v>1118668575</v>
@@ -619,19 +619,19 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>44749.79125</v>
+        <v>44671.79125</v>
       </c>
       <c r="B10">
-        <v>2430</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Mensualidad Julio 2022</v>
-      </c>
-      <c r="D10">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="C10">
+        <v>4673</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Mensualidad Abril 2022</v>
       </c>
       <c r="E10" t="str">
-        <v>10050</v>
+        <v>8434</v>
       </c>
       <c r="F10" t="str">
         <v>1118668575</v>
@@ -642,19 +642,19 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>44773.79125</v>
+        <v>44671.79125</v>
       </c>
       <c r="B11">
-        <v>19840</v>
-      </c>
-      <c r="C11" t="str">
-        <v>Mensualidad Agosto 2022 - Marzo 2023</v>
-      </c>
-      <c r="D11">
-        <v>23</v>
+        <v>37</v>
+      </c>
+      <c r="C11">
+        <v>3608</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Mensualidad Abril 2022</v>
       </c>
       <c r="E11" t="str">
-        <v>10505</v>
+        <v>8433</v>
       </c>
       <c r="F11" t="str">
         <v>1118668575</v>
@@ -665,19 +665,19 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>45016.74958333333</v>
+        <v>44699.79125</v>
       </c>
       <c r="B12">
-        <v>17010</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Mensualidad Abril 2023 - Octubre 2023</v>
-      </c>
-      <c r="D12">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="C12">
+        <v>3608</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Mensualidad Mayo 2022</v>
       </c>
       <c r="E12" t="str">
-        <v>10525</v>
+        <v>9066</v>
       </c>
       <c r="F12" t="str">
         <v>1118668575</v>
@@ -688,19 +688,19 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>45230.74958333333</v>
+        <v>44727.79125</v>
       </c>
       <c r="B13">
-        <v>48600</v>
-      </c>
-      <c r="C13" t="str">
-        <v>Mensualidad 38 a la 58</v>
-      </c>
-      <c r="D13">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="C13">
+        <v>3608</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Mensualidad Junio 2022</v>
       </c>
       <c r="E13" t="str">
-        <v>11077</v>
+        <v>9560</v>
       </c>
       <c r="F13" t="str">
         <v>1118668575</v>
@@ -711,35 +711,417 @@
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>45166.74958333333</v>
+        <v>44699.79125</v>
       </c>
       <c r="B14">
-        <v>4860</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Mensualidad 59 y 60</v>
-      </c>
-      <c r="D14">
-        <v>59</v>
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>4673</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Mensualidad Mayo 2022</v>
       </c>
       <c r="E14" t="str">
-        <v/>
+        <v>9067</v>
       </c>
       <c r="F14" t="str">
-        <v/>
+        <v>1118668575</v>
       </c>
       <c r="G14" t="str">
-        <v>Se toman saldos a favor</v>
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>44727.79125</v>
+      </c>
+      <c r="B15">
+        <v>36</v>
+      </c>
+      <c r="C15">
+        <v>4673</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Mensualidad Junio 2022</v>
+      </c>
+      <c r="E15" t="str">
+        <v>9562</v>
+      </c>
+      <c r="F15" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G15" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>44761.79125</v>
+      </c>
+      <c r="B16">
+        <v>37</v>
+      </c>
+      <c r="C16">
+        <v>4673</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Mensualidad Julio 2022</v>
+      </c>
+      <c r="E16" t="str">
+        <v>10378</v>
+      </c>
+      <c r="F16" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G16" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>44761.79125</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>3608</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Mensualidad Julio 2022</v>
+      </c>
+      <c r="E17" t="str">
+        <v>10377</v>
+      </c>
+      <c r="F17" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G17" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>44790.79125</v>
+      </c>
+      <c r="B18">
+        <v>41</v>
+      </c>
+      <c r="C18">
+        <v>3608</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Mensualidad Agosto 2022</v>
+      </c>
+      <c r="E18" t="str">
+        <v>10998</v>
+      </c>
+      <c r="F18" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G18" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>44790.79125</v>
+      </c>
+      <c r="B19">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>4673</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Mensualidad Agosto 2022</v>
+      </c>
+      <c r="E19" t="str">
+        <v>10999</v>
+      </c>
+      <c r="F19" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G19" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>44822.79125</v>
+      </c>
+      <c r="B20">
+        <v>39</v>
+      </c>
+      <c r="C20">
+        <v>4673</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Mensualidad Septiembre 2022</v>
+      </c>
+      <c r="E20" t="str">
+        <v>11492</v>
+      </c>
+      <c r="F20" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G20" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>44822.79125</v>
+      </c>
+      <c r="B21">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>3608</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Mensualidad Septiembre 2022</v>
+      </c>
+      <c r="E21" t="str">
+        <v>11491</v>
+      </c>
+      <c r="F21" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G21" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>44853.79125</v>
+      </c>
+      <c r="B22">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>4673</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Mensualidad Octubre 2022</v>
+      </c>
+      <c r="E22" t="str">
+        <v>12145</v>
+      </c>
+      <c r="F22" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G22" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>44853.79125</v>
+      </c>
+      <c r="B23">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>3608</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Mensualidad Octubre 2022</v>
+      </c>
+      <c r="E23" t="str">
+        <v>12144</v>
+      </c>
+      <c r="F23" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G23" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>44885.74958333333</v>
+      </c>
+      <c r="B24">
+        <v>41</v>
+      </c>
+      <c r="C24">
+        <v>4673</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Mensualidad Noviembre 2022</v>
+      </c>
+      <c r="E24" t="str">
+        <v>12663</v>
+      </c>
+      <c r="F24" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G24" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>44885.74958333333</v>
+      </c>
+      <c r="B25">
+        <v>44</v>
+      </c>
+      <c r="C25">
+        <v>3608</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Mensualidad Noviembre 2022</v>
+      </c>
+      <c r="E25" t="str">
+        <v>12662</v>
+      </c>
+      <c r="F25" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G25" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>44913.74958333333</v>
+      </c>
+      <c r="B26">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <v>4673</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Mensualidad Diciembre 2022</v>
+      </c>
+      <c r="E26" t="str">
+        <v>13276</v>
+      </c>
+      <c r="F26" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G26" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>44913.74958333333</v>
+      </c>
+      <c r="B27">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>3608</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Mensualidad Diciembre 2022</v>
+      </c>
+      <c r="E27" t="str">
+        <v>13275</v>
+      </c>
+      <c r="F27" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G27" t="str">
+        <v>BANORTE/IXE</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G27"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>fecha</v>
+      </c>
+      <c r="B1" t="str">
+        <v>mensualidad</v>
+      </c>
+      <c r="C1" t="str">
+        <v>refPago</v>
+      </c>
+      <c r="D1" t="str">
+        <v>folio</v>
+      </c>
+      <c r="E1" t="str">
+        <v>refBanco</v>
+      </c>
+      <c r="F1" t="str">
+        <v>ctaBancaria</v>
+      </c>
+      <c r="G1" t="str">
+        <v>banco</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>45266.74958333333</v>
+      </c>
+      <c r="B2">
+        <v>46730</v>
+      </c>
+      <c r="C2" t="str">
+        <v>MENSUALIDAD 43 A LA 52</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <v>BANORTE</v>
+      </c>
+      <c r="F2" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G2" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>45266.74958333333</v>
+      </c>
+      <c r="B3">
+        <v>25256</v>
+      </c>
+      <c r="C3" t="str">
+        <v>MENSUALIDAD 46 A LA 52</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>BANORTE</v>
+      </c>
+      <c r="F3" t="str">
+        <v>1118668575</v>
+      </c>
+      <c r="G3" t="str">
+        <v>BANORTE/IXE</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
@@ -752,9 +1134,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -784,265 +1166,35 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>44501.74958333333</v>
+        <v>44544.74958333333</v>
       </c>
       <c r="B2">
-        <v>243</v>
+        <v>4673</v>
       </c>
       <c r="C2" t="str">
-        <v>mora noviembre</v>
+        <v>Abarca hasta  noviembre</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="str">
-        <v>5687</v>
-      </c>
-      <c r="F2" t="str">
-        <v>1118668575</v>
-      </c>
-      <c r="G2" t="str">
-        <v>BANORTE/IXE</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>44542.74958333333</v>
+        <v>44544.74958333333</v>
       </c>
       <c r="B3">
-        <v>243</v>
+        <v>3608</v>
       </c>
       <c r="C3" t="str">
-        <v>saldo a favor</v>
+        <v>Abarca hasta  noviembre</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="str">
-        <v>5687</v>
-      </c>
-      <c r="F3" t="str">
-        <v>1118668575</v>
-      </c>
-      <c r="G3" t="str">
-        <v>BANORTE/IXE</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>44616.74958333333</v>
-      </c>
-      <c r="B4">
-        <v>570</v>
-      </c>
-      <c r="C4" t="str">
-        <v>saldo a favor</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="str">
-        <v>7211</v>
-      </c>
-      <c r="F4" t="str">
-        <v>1118668575</v>
-      </c>
-      <c r="G4" t="str">
-        <v>BANORTE/IXE</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>44676.79125</v>
-      </c>
-      <c r="B5">
-        <v>243</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Mora Abril 2022</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="str">
-        <v>9142</v>
-      </c>
-      <c r="F5" t="str">
-        <v>1118668575</v>
-      </c>
-      <c r="G5" t="str">
-        <v>BANORTE/IXE</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>44706.79125</v>
-      </c>
-      <c r="B6">
-        <v>243</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Mora Mayo 2022</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="str">
-        <v>9142</v>
-      </c>
-      <c r="F6" t="str">
-        <v>1118668575</v>
-      </c>
-      <c r="G6" t="str">
-        <v>BANORTE/IXE</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1">
-        <v>44741.79125</v>
-      </c>
-      <c r="B7">
-        <v>243</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Mora Junio 2022</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7" t="str">
-        <v>10050</v>
-      </c>
-      <c r="F7" t="str">
-        <v>1118668575</v>
-      </c>
-      <c r="G7" t="str">
-        <v>BANORTE/IXE</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1">
-        <v>44768.79125</v>
-      </c>
-      <c r="B8">
-        <v>790</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Saldo a Favor Deposito Julio</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8" t="str">
-        <v>10505</v>
-      </c>
-      <c r="F8" t="str">
-        <v>1118668575</v>
-      </c>
-      <c r="G8" t="str">
-        <v>BANORTE/IXE</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1">
-        <v>44767.79125</v>
-      </c>
-      <c r="B9">
-        <v>490</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Saldo a Favor Deposito Julio</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9" t="str">
-        <v>10525</v>
-      </c>
-      <c r="F9" t="str">
-        <v>1118668575</v>
-      </c>
-      <c r="G9" t="str">
-        <v>BANORTE/IXE</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1">
-        <v>44801.79125</v>
-      </c>
-      <c r="B10">
-        <v>1400</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Saldo a Favor Deposito Agosto</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10" t="str">
-        <v>11077</v>
-      </c>
-      <c r="F10" t="str">
-        <v>1118668575</v>
-      </c>
-      <c r="G10" t="str">
-        <v>BANORTE/IXE</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G10"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>fecha</v>
-      </c>
-      <c r="B1" t="str">
-        <v>mensualidad</v>
-      </c>
-      <c r="C1" t="str">
-        <v>refPago</v>
-      </c>
-      <c r="D1" t="str">
-        <v>folio</v>
-      </c>
-      <c r="E1" t="str">
-        <v>refBanco</v>
-      </c>
-      <c r="F1" t="str">
-        <v>ctaBancaria</v>
-      </c>
-      <c r="G1" t="str">
-        <v>banco</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>44542.74958333333</v>
-      </c>
-      <c r="B2">
-        <v>2430</v>
-      </c>
-      <c r="C2" t="str">
-        <v>abarca hasta octubre</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1073,10 +1225,10 @@
     </row>
     <row r="2">
       <c r="B2" t="str">
-        <v>JAVIER ALBERTO GUTIERREZ GOMEZ</v>
+        <v>JORGE AARON ALCAZAR VILLEGAS</v>
       </c>
       <c r="C2" t="str">
-        <v>javieralbertogutierrezgomez@gmail.com</v>
+        <v>jorgeaaronalcazarvillegas@gmail.com</v>
       </c>
       <c r="D2" t="str">
         <v>No Data</v>
@@ -1112,7 +1264,7 @@
     </row>
     <row r="2">
       <c r="B2" t="str">
-        <v>KUXTAL 3</v>
+        <v>YA'AX BEH</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1184,28 +1336,28 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F2" t="str">
-        <v>3</v>
+        <v/>
       </c>
       <c r="G2">
-        <v>171562</v>
+        <v>270000</v>
       </c>
       <c r="H2">
-        <v>25734</v>
+        <v>27000</v>
       </c>
       <c r="I2">
-        <v>145827</v>
+        <v>243000</v>
       </c>
       <c r="J2">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K2">
-        <v>2430</v>
+        <v>4673</v>
       </c>
       <c r="L2" s="1">
-        <v>44118.79125</v>
+        <v>43691.79125</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1244,19 +1396,19 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>4465</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>112180</v>
+        <v>107653</v>
       </c>
       <c r="C2">
-        <v>2430</v>
+        <v>8281</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>71986</v>
       </c>
       <c r="E2">
-        <v>114610</v>
+        <v>187920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>